<commit_message>
Backup on 2026-02-18 08:52:25
</commit_message>
<xml_diff>
--- a/erp_summary.xlsx
+++ b/erp_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timmcmullin/Documents/Python/coop research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{526E9E21-0CAB-324B-80A5-B1BE660BAA44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{791EF2D6-89AD-6246-B36D-1D6D25DF091C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17420" xr2:uid="{C7A39DAA-EA55-3841-A75A-7B54E01839E3}"/>
   </bookViews>
@@ -278,7 +278,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -413,8 +413,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -592,6 +600,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -711,7 +725,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -754,11 +768,14 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -792,6 +809,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1134,9 +1152,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBC4FECD-E045-3741-87DB-7A82F677654B}">
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="53" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1163,156 +1188,168 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2">
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="F2">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="D3">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="F3">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="F4">
         <v>0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="G5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
       <c r="C6">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="D6">
         <v>10</v>
       </c>
       <c r="E6">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="F6">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="G7" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="G8" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
@@ -1324,10 +1361,10 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G9" t="s">
         <v>8</v>
@@ -1335,70 +1372,76 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>50</v>
+      </c>
+      <c r="G10" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="G11" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
       </c>
       <c r="C12">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="D12">
         <v>10</v>
       </c>
       <c r="E12">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="F12">
         <v>10</v>
       </c>
       <c r="G12" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="B13" t="s">
         <v>4</v>
@@ -1413,41 +1456,44 @@
         <v>90</v>
       </c>
       <c r="F13">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G13" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="G14" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="B15" t="s">
         <v>4</v>
       </c>
       <c r="C15">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="D15">
         <v>10</v>
@@ -1456,7 +1502,7 @@
         <v>90</v>
       </c>
       <c r="F15">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G15" t="s">
         <v>26</v>
@@ -1464,27 +1510,30 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="G16" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="B17" t="s">
         <v>4</v>
@@ -1493,13 +1542,13 @@
         <v>0.9</v>
       </c>
       <c r="D17">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E17">
         <v>90</v>
       </c>
       <c r="F17">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G17" t="s">
         <v>8</v>
@@ -1507,13 +1556,13 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>69</v>
       </c>
       <c r="B18" t="s">
         <v>4</v>
       </c>
       <c r="C18">
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
       <c r="D18">
         <v>10</v>
@@ -1522,15 +1571,15 @@
         <v>90</v>
       </c>
       <c r="F18">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G18" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="B19" t="s">
         <v>4</v>
@@ -1545,7 +1594,7 @@
         <v>90</v>
       </c>
       <c r="F19">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G19" t="s">
         <v>8</v>
@@ -1553,7 +1602,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>76</v>
       </c>
       <c r="B20" t="s">
         <v>4</v>
@@ -1562,27 +1611,27 @@
         <v>0.9</v>
       </c>
       <c r="D20">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E20">
         <v>90</v>
       </c>
       <c r="F20">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="G20" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>79</v>
       </c>
       <c r="B21" t="s">
         <v>4</v>
       </c>
       <c r="C21">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="D21">
         <v>10</v>
@@ -1591,15 +1640,15 @@
         <v>90</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G21" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B22" t="s">
         <v>4</v>
@@ -1614,110 +1663,113 @@
         <v>90</v>
       </c>
       <c r="F22">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="G22" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B23" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>0.85</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="G23" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="B24" t="s">
         <v>4</v>
       </c>
       <c r="C24">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E24">
         <v>90</v>
       </c>
       <c r="F24">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G24" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="B25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C25">
-        <v>0.95</v>
+        <v>0.85</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E25">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="F25">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="G25" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="B26" t="s">
         <v>4</v>
       </c>
       <c r="C26">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="D26">
         <v>10</v>
       </c>
       <c r="E26">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="F26">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="G26" t="s">
-        <v>41</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
         <v>4</v>
       </c>
       <c r="C27">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="D27">
         <v>10</v>
@@ -1726,15 +1778,15 @@
         <v>90</v>
       </c>
       <c r="F27">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G27" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B28" t="s">
         <v>4</v>
@@ -1746,64 +1798,67 @@
         <v>10</v>
       </c>
       <c r="E28">
+        <v>90</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="D29" s="2">
+        <v>10</v>
+      </c>
+      <c r="E29" s="2">
         <v>80</v>
       </c>
-      <c r="F28">
+      <c r="F29" s="2">
         <v>50</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G29" s="2" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>45</v>
-      </c>
-      <c r="B29" t="s">
-        <v>12</v>
-      </c>
-      <c r="C29">
-        <v>0.1</v>
-      </c>
-      <c r="D29">
-        <v>10</v>
-      </c>
-      <c r="E29">
-        <v>5</v>
-      </c>
-      <c r="F29">
-        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B30" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C30">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="D30">
         <v>10</v>
       </c>
       <c r="E30">
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="F30">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="G30" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B31" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C31">
         <v>0.8</v>
@@ -1812,24 +1867,24 @@
         <v>10</v>
       </c>
       <c r="E31">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="F31">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="G31" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="B32" t="s">
         <v>4</v>
       </c>
       <c r="C32">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="D32">
         <v>10</v>
@@ -1838,35 +1893,38 @@
         <v>90</v>
       </c>
       <c r="F32">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="G32" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="B33" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="D33">
         <v>0</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="F33">
-        <v>0</v>
+        <v>50</v>
+      </c>
+      <c r="G33" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="B34" t="s">
         <v>4</v>
@@ -1875,105 +1933,108 @@
         <v>0.8</v>
       </c>
       <c r="D34">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E34">
         <v>80</v>
       </c>
       <c r="F34">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G34" t="s">
-        <v>53</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>54</v>
+        <v>81</v>
       </c>
       <c r="B35" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="D35">
         <v>0</v>
       </c>
       <c r="E35">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="F35">
         <v>0</v>
+      </c>
+      <c r="G35" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="B36" t="s">
         <v>4</v>
       </c>
       <c r="C36">
-        <v>0.85</v>
+        <v>0.75</v>
       </c>
       <c r="D36">
         <v>10</v>
       </c>
       <c r="E36">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="F36">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G36" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="B37" t="s">
         <v>4</v>
       </c>
       <c r="C37">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
       <c r="D37">
         <v>10</v>
       </c>
       <c r="E37">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="F37">
         <v>5</v>
       </c>
       <c r="G37" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="B38" t="s">
         <v>4</v>
       </c>
       <c r="C38">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="D38">
         <v>10</v>
       </c>
       <c r="E38">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="F38">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G38" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -2001,122 +2062,107 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B40" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C40">
-        <v>0.8</v>
+        <v>0.1</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E40">
-        <v>90</v>
+        <v>5</v>
       </c>
       <c r="F40">
-        <v>50</v>
-      </c>
-      <c r="G40" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="B41" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C41">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="D41">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E41">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="F41">
-        <v>30</v>
-      </c>
-      <c r="G41" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="B42" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C42">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="D42">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E42">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="F42">
-        <v>10</v>
-      </c>
-      <c r="G42" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="B43" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C43">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="D43">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E43">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="F43">
-        <v>30</v>
-      </c>
-      <c r="G43" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>65</v>
+        <v>16</v>
       </c>
       <c r="B44" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C44">
-        <v>0.85</v>
+        <v>0</v>
       </c>
       <c r="D44">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E44">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="F44">
-        <v>50</v>
-      </c>
-      <c r="G44" t="s">
-        <v>43</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>66</v>
+        <v>18</v>
       </c>
       <c r="B45" t="s">
         <v>12</v>
@@ -2136,30 +2182,27 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>67</v>
+        <v>19</v>
       </c>
       <c r="B46" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C46">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="D46">
         <v>0</v>
       </c>
       <c r="E46">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="F46">
         <v>0</v>
-      </c>
-      <c r="G46" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>68</v>
+        <v>24</v>
       </c>
       <c r="B47" t="s">
         <v>12</v>
@@ -2179,76 +2222,67 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>69</v>
+        <v>27</v>
       </c>
       <c r="B48" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C48">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="D48">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E48">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="F48">
-        <v>10</v>
-      </c>
-      <c r="G48" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="B49" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C49">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="D49">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E49">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="F49">
-        <v>10</v>
-      </c>
-      <c r="G49" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="B50" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C50">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="D50">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E50">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="F50">
-        <v>30</v>
-      </c>
-      <c r="G50" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="B51" t="s">
         <v>12</v>
@@ -2266,9 +2300,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B52" t="s">
         <v>12</v>
@@ -2286,9 +2320,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B53" t="s">
         <v>12</v>
@@ -2306,9 +2340,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B54" t="s">
         <v>12</v>
@@ -2326,32 +2360,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B55" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C55">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="D55">
         <v>0</v>
       </c>
       <c r="E55">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="F55">
-        <v>70</v>
-      </c>
-      <c r="G55" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B56" t="s">
         <v>12</v>
@@ -2369,53 +2400,47 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B57" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C57">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="D57">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E57">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="F57">
-        <v>50</v>
-      </c>
-      <c r="G57" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B58" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C58">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="D58">
         <v>0</v>
       </c>
       <c r="E58">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="F58">
         <v>0</v>
       </c>
-      <c r="G58" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>82</v>
       </c>
@@ -2435,7 +2460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>83</v>
       </c>
@@ -2456,6 +2481,12 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G60">
+    <sortCondition descending="1" ref="C2:C60"/>
+  </sortState>
+  <hyperlinks>
+    <hyperlink ref="G28" r:id="rId1" xr:uid="{0E4A9DD0-DA1C-AE4C-926C-B991036FBFFB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>